<commit_message>
corrected typos in Supplementary Data Set 4
</commit_message>
<xml_diff>
--- a/data_20170315/Supplementary_Data_Sets/Supplementary_Data_Set_4.xlsx
+++ b/data_20170315/Supplementary_Data_Sets/Supplementary_Data_Set_4.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="0" windowWidth="25120" windowHeight="15580" tabRatio="705"/>
@@ -102,9 +102,6 @@
     <t>(YGL200C, YGL170C)</t>
   </si>
   <si>
-    <t>ANC(UFRJ50876, YPS138)</t>
-  </si>
-  <si>
     <t>(YFR012W, YFR028C)</t>
   </si>
   <si>
@@ -175,9 +172,6 @@
   </si>
   <si>
     <t>UWOPS91-917.1</t>
-  </si>
-  <si>
-    <t>ANC(UWOPS91-917.1, (UFRJ50876, YPS138))</t>
   </si>
   <si>
     <t>UWOPS03-461.4</t>
@@ -814,6 +808,12 @@
   </si>
   <si>
     <t xml:space="preserve">Supplementary Data Set 4: Balanced rearrangement events identified in the 12 strains. </t>
+  </si>
+  <si>
+    <t>ANC(UFRJ50816, YPS138)</t>
+  </si>
+  <si>
+    <t>ANC(UWOPS91-917.1, (UFRJ50816, YPS138))</t>
   </si>
 </sst>
 </file>
@@ -3470,7 +3470,7 @@
   <dimension ref="A1:X73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A2" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3489,7 +3489,7 @@
   <sheetData>
     <row r="1" spans="1:24" s="6" customFormat="1">
       <c r="A1" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -3498,22 +3498,22 @@
     </row>
     <row r="2" spans="1:24">
       <c r="A2" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>42</v>
-      </c>
       <c r="C2" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
@@ -3522,29 +3522,29 @@
       <c r="K2" s="16"/>
       <c r="L2" s="16"/>
       <c r="M2" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N2" s="16"/>
       <c r="O2" s="16"/>
       <c r="P2" s="16"/>
       <c r="Q2" s="16"/>
       <c r="R2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U2" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="V2" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="T2" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="U2" s="8" t="s">
+      <c r="W2" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="V2" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="W2" s="7" t="s">
-        <v>68</v>
       </c>
       <c r="X2" s="17" t="s">
         <v>5</v>
@@ -3557,58 +3557,58 @@
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="8" t="s">
+      <c r="K3" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="L3" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="M3" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>74</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>2</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="Q3" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="S3" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="T3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="U3" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="T3" s="9" t="s">
+      <c r="V3" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="U3" s="8" t="s">
+      <c r="W3" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="V3" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="W3" s="8" t="s">
-        <v>82</v>
       </c>
       <c r="X3" s="17"/>
     </row>
@@ -3623,7 +3623,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>7</v>
@@ -3683,7 +3683,7 @@
         <v>0</v>
       </c>
       <c r="X4" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -3697,7 +3697,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>7</v>
@@ -3757,7 +3757,7 @@
         <v>0</v>
       </c>
       <c r="X5" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:24">
@@ -3765,13 +3765,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>7</v>
@@ -3831,7 +3831,7 @@
         <v>0</v>
       </c>
       <c r="X6" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:24">
@@ -3839,16 +3839,16 @@
         <v>4</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
@@ -3863,7 +3863,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K8" s="2">
         <v>0</v>
@@ -3878,34 +3878,34 @@
         <v>0</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Q8" s="2">
         <v>0</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="X8" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -3919,10 +3919,10 @@
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
@@ -3937,7 +3937,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K9" s="2">
         <v>0</v>
@@ -3952,34 +3952,34 @@
         <v>0</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Q9" s="2">
         <v>0</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="X9" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:24">
@@ -3987,13 +3987,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>8</v>
@@ -4058,16 +4058,16 @@
         <v>7</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" s="2">
         <v>0</v>
@@ -4129,10 +4129,10 @@
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="2">
         <v>0</v>
@@ -4194,10 +4194,10 @@
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
@@ -4259,10 +4259,10 @@
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F16" s="2">
         <v>0</v>
@@ -4324,10 +4324,10 @@
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F17" s="2">
         <v>0</v>
@@ -4395,7 +4395,7 @@
         <v>6</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>10</v>
@@ -4455,7 +4455,7 @@
         <v>0</v>
       </c>
       <c r="X19" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:24">
@@ -4475,7 +4475,7 @@
         <v>6</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>12</v>
@@ -4535,7 +4535,7 @@
         <v>0</v>
       </c>
       <c r="X21" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:24">
@@ -4549,7 +4549,7 @@
         <v>6</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>12</v>
@@ -4609,7 +4609,7 @@
         <v>0</v>
       </c>
       <c r="X22" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:24">
@@ -4617,13 +4617,13 @@
         <v>11</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>22</v>
@@ -4683,7 +4683,7 @@
         <v>0</v>
       </c>
       <c r="X23" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:24">
@@ -4703,7 +4703,7 @@
         <v>6</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>11</v>
@@ -4763,7 +4763,7 @@
         <v>0</v>
       </c>
       <c r="X25" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:24">
@@ -4771,16 +4771,16 @@
         <v>13</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F26" s="2">
         <v>0</v>
@@ -4837,7 +4837,7 @@
         <v>0</v>
       </c>
       <c r="X26" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:24">
@@ -4851,7 +4851,7 @@
         <v>6</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>25</v>
@@ -4911,7 +4911,7 @@
         <v>0</v>
       </c>
       <c r="X28" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:24">
@@ -4919,13 +4919,13 @@
         <v>15</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>26</v>
@@ -4990,13 +4990,13 @@
         <v>16</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>20</v>
@@ -5061,13 +5061,13 @@
         <v>17</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>21</v>
@@ -5127,7 +5127,7 @@
         <v>0</v>
       </c>
       <c r="X34" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:24">
@@ -5141,10 +5141,10 @@
         <v>6</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F36" s="2">
         <v>0</v>
@@ -5212,7 +5212,7 @@
         <v>6</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>15</v>
@@ -5283,7 +5283,7 @@
         <v>6</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>14</v>
@@ -5354,7 +5354,7 @@
         <v>6</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>18</v>
@@ -5431,10 +5431,10 @@
         <v>6</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F44" s="2">
         <v>0</v>
@@ -5502,7 +5502,7 @@
         <v>6</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>17</v>
@@ -5573,7 +5573,7 @@
         <v>6</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>16</v>
@@ -5644,7 +5644,7 @@
         <v>6</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>13</v>
@@ -5704,7 +5704,7 @@
         <v>0</v>
       </c>
       <c r="X49" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:24">
@@ -5718,10 +5718,10 @@
         <v>6</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F51" s="2">
         <v>0</v>
@@ -5789,10 +5789,10 @@
         <v>6</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F52" s="2">
         <v>0</v>
@@ -5854,16 +5854,16 @@
         <v>28</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F54" s="2">
         <v>0</v>
@@ -5920,7 +5920,7 @@
         <v>0</v>
       </c>
       <c r="X54" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="1:24">
@@ -5934,13 +5934,13 @@
         <v>29</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>23</v>
@@ -5982,25 +5982,25 @@
         <v>1</v>
       </c>
       <c r="R56" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="S56" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="T56" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="U56" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="V56" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="W56" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="X56" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="58" spans="1:24">
@@ -6014,10 +6014,10 @@
         <v>19</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F58" s="2">
         <v>0</v>
@@ -6091,10 +6091,10 @@
         <v>19</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F60" s="2">
         <v>0</v>
@@ -6168,10 +6168,10 @@
         <v>19</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F62" s="2">
         <v>0</v>
@@ -6245,10 +6245,10 @@
         <v>19</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F64" s="2">
         <v>0</v>
@@ -6322,10 +6322,10 @@
         <v>19</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E66" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F66" s="2">
         <v>0</v>
@@ -6387,16 +6387,16 @@
         <v>35</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C68" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F68" s="4">
         <v>0</v>
@@ -6461,22 +6461,22 @@
     </row>
     <row r="70" spans="1:24">
       <c r="A70" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="71" spans="1:24">
       <c r="A71" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="72" spans="1:24">
       <c r="A72" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="73" spans="1:24">
       <c r="A73" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>